<commit_message>
More Updates Test and SeleniumUtil
</commit_message>
<xml_diff>
--- a/SeleniumPjt/TestData/TestDataExcel.xlsx
+++ b/SeleniumPjt/TestData/TestDataExcel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestConfiguration" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="40">
   <si>
     <t>Execute</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>promoCodeTest</t>
+  </si>
+  <si>
+    <t>CheckWelcomeMessage</t>
+  </si>
+  <si>
+    <t>Welcome to Shoe Store!</t>
   </si>
 </sst>
 </file>
@@ -547,10 +553,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,6 +613,14 @@
         <v>36</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -617,7 +631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17:B21"/>
     </sheetView>
   </sheetViews>

</xml_diff>